<commit_message>
Fix procedures. Add data from sponser. Created logic for scheduling weekdays. Ready for API test. Need Shift Preferences from sponser or make rands.
</commit_message>
<xml_diff>
--- a/Barton1792DB/Barton1792DB/Barton1792DB/bin/DataFiles/Copy of MASTER SENIORITY LISTING.xlsx
+++ b/Barton1792DB/Barton1792DB/Barton1792DB/bin/DataFiles/Copy of MASTER SENIORITY LISTING.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Telahun\Documents\School\CECS596\Barton1792\Barton1792API\BartonAPI\Barton1792DB\Barton1792DB\Barton1792DB\bin\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02F7AAF-D855-4E7D-BA67-7BCEF1E22B9E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5F1DA1-DD7B-47F0-983C-4D8644A09E28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6240" yWindow="915" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2795" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2731" uniqueCount="829">
   <si>
     <t>EMPLOYEE NAME</t>
   </si>
@@ -2665,7 +2665,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2824,6 +2824,20 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18295,19 +18309,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37244190-D222-4663-AC6D-2030567E4A09}">
-  <dimension ref="A1:O303"/>
+  <dimension ref="A1:O304"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
+      <selection activeCell="H301" sqref="H301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="40.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" customWidth="1"/>
+    <col min="14" max="14" width="30.7109375" customWidth="1"/>
     <col min="15" max="15" width="79.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="162" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>518</v>
       </c>
@@ -18361,7 +18388,7 @@
       <c r="B2" s="4">
         <v>1977</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="51">
         <v>28396</v>
       </c>
       <c r="D2" s="22">
@@ -18409,8 +18436,8 @@
       <c r="B3" s="4">
         <v>1977</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>12</v>
+      <c r="C3" s="51">
+        <v>28401</v>
       </c>
       <c r="D3" s="22">
         <v>43466</v>
@@ -18457,7 +18484,7 @@
       <c r="B4" s="4">
         <v>1977</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="51">
         <v>28402</v>
       </c>
       <c r="D4" s="22">
@@ -18505,7 +18532,7 @@
       <c r="B5" s="4">
         <v>1977</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="51">
         <v>28411</v>
       </c>
       <c r="D5" s="22">
@@ -18553,8 +18580,8 @@
       <c r="B6" s="4">
         <v>1978</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>244</v>
+      <c r="C6" s="52">
+        <v>28705</v>
       </c>
       <c r="D6" s="22">
         <v>43466</v>
@@ -18601,8 +18628,8 @@
       <c r="B7" s="4">
         <v>1978</v>
       </c>
-      <c r="C7" s="31" t="s">
-        <v>244</v>
+      <c r="C7" s="53">
+        <v>28705</v>
       </c>
       <c r="D7" s="22">
         <v>43466</v>
@@ -18649,7 +18676,7 @@
       <c r="B8" s="4">
         <v>1978</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="54">
         <v>28795</v>
       </c>
       <c r="D8" s="22">
@@ -18697,8 +18724,8 @@
       <c r="B9" s="4">
         <v>1979</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>245</v>
+      <c r="C9" s="53">
+        <v>28878</v>
       </c>
       <c r="D9" s="22">
         <v>43466</v>
@@ -18745,7 +18772,7 @@
       <c r="B10" s="4">
         <v>1979</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="51">
         <v>28879</v>
       </c>
       <c r="D10" s="22">
@@ -18793,7 +18820,7 @@
       <c r="B11" s="4">
         <v>1979</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="51">
         <v>28961</v>
       </c>
       <c r="D11" s="22">
@@ -18841,8 +18868,8 @@
       <c r="B12" s="4">
         <v>1979</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>246</v>
+      <c r="C12" s="51">
+        <v>28961</v>
       </c>
       <c r="D12" s="22">
         <v>43466</v>
@@ -18889,8 +18916,8 @@
       <c r="B13" s="4">
         <v>1979</v>
       </c>
-      <c r="C13" s="31" t="s">
-        <v>246</v>
+      <c r="C13" s="53">
+        <v>28961</v>
       </c>
       <c r="D13" s="22">
         <v>43466</v>
@@ -18937,7 +18964,7 @@
       <c r="B14" s="4">
         <v>1979</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="51">
         <v>29017</v>
       </c>
       <c r="D14" s="22">
@@ -18985,7 +19012,7 @@
       <c r="B15" s="4">
         <v>1979</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="51">
         <v>29017</v>
       </c>
       <c r="D15" s="22">
@@ -19033,8 +19060,8 @@
       <c r="B16" s="4">
         <v>1979</v>
       </c>
-      <c r="C16" s="31" t="s">
-        <v>280</v>
+      <c r="C16" s="53">
+        <v>28996</v>
       </c>
       <c r="D16" s="22">
         <v>43466</v>
@@ -19081,8 +19108,8 @@
       <c r="B17" s="4">
         <v>1979</v>
       </c>
-      <c r="C17" s="31" t="s">
-        <v>280</v>
+      <c r="C17" s="53">
+        <v>28996</v>
       </c>
       <c r="D17" s="22">
         <v>43466</v>
@@ -19129,8 +19156,8 @@
       <c r="B18" s="4">
         <v>1980</v>
       </c>
-      <c r="C18" s="31" t="s">
-        <v>247</v>
+      <c r="C18" s="53">
+        <v>29327</v>
       </c>
       <c r="D18" s="22">
         <v>43466</v>
@@ -19177,7 +19204,7 @@
       <c r="B19" s="4">
         <v>1980</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="51">
         <v>29333</v>
       </c>
       <c r="D19" s="22">
@@ -19225,7 +19252,7 @@
       <c r="B20" s="4">
         <v>1980</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="51">
         <v>29333</v>
       </c>
       <c r="D20" s="22">
@@ -19273,7 +19300,7 @@
       <c r="B21" s="4">
         <v>1980</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="51">
         <v>29336</v>
       </c>
       <c r="D21" s="22">
@@ -19321,7 +19348,7 @@
       <c r="B22" s="4">
         <v>1980</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="51">
         <v>29348</v>
       </c>
       <c r="D22" s="22">
@@ -19369,7 +19396,7 @@
       <c r="B23" s="4">
         <v>1980</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="51">
         <v>29361</v>
       </c>
       <c r="D23" s="22">
@@ -19417,8 +19444,8 @@
       <c r="B24" s="4">
         <v>1980</v>
       </c>
-      <c r="C24" s="31" t="s">
-        <v>42</v>
+      <c r="C24" s="53">
+        <v>29503</v>
       </c>
       <c r="D24" s="22">
         <v>43466</v>
@@ -19465,7 +19492,7 @@
       <c r="B25" s="4">
         <v>1980</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="51">
         <v>29504</v>
       </c>
       <c r="D25" s="22">
@@ -19513,8 +19540,8 @@
       <c r="B26" s="4">
         <v>1980</v>
       </c>
-      <c r="C26" s="31" t="s">
-        <v>46</v>
+      <c r="C26" s="53">
+        <v>29518</v>
       </c>
       <c r="D26" s="22">
         <v>43466</v>
@@ -19561,7 +19588,7 @@
       <c r="B27" s="4">
         <v>1981</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="51">
         <v>29850</v>
       </c>
       <c r="D27" s="22">
@@ -19609,8 +19636,8 @@
       <c r="B28" s="4">
         <v>1989</v>
       </c>
-      <c r="C28" s="31" t="s">
-        <v>50</v>
+      <c r="C28" s="53">
+        <v>32808</v>
       </c>
       <c r="D28" s="22">
         <v>43466</v>
@@ -19657,7 +19684,7 @@
       <c r="B29" s="4">
         <v>1990</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="51">
         <v>33127</v>
       </c>
       <c r="D29" s="22">
@@ -19705,7 +19732,7 @@
       <c r="B30" s="4">
         <v>1990</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="54">
         <v>33133</v>
       </c>
       <c r="D30" s="22">
@@ -19753,7 +19780,7 @@
       <c r="B31" s="4">
         <v>1990</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="51">
         <v>33133</v>
       </c>
       <c r="D31" s="22">
@@ -19801,7 +19828,7 @@
       <c r="B32" s="4">
         <v>1990</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="51">
         <v>33203</v>
       </c>
       <c r="D32" s="22">
@@ -19849,7 +19876,7 @@
       <c r="B33" s="4">
         <v>1996</v>
       </c>
-      <c r="C33" s="22">
+      <c r="C33" s="51">
         <v>35177</v>
       </c>
       <c r="D33" s="22">
@@ -19897,7 +19924,7 @@
       <c r="B34" s="4">
         <v>1996</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C34" s="52">
         <v>35285</v>
       </c>
       <c r="D34" s="22">
@@ -19945,8 +19972,8 @@
       <c r="B35" s="4">
         <v>1996</v>
       </c>
-      <c r="C35" s="31" t="s">
-        <v>64</v>
+      <c r="C35" s="53">
+        <v>35296</v>
       </c>
       <c r="D35" s="22">
         <v>43466</v>
@@ -19993,7 +20020,7 @@
       <c r="B36" s="4">
         <v>1996</v>
       </c>
-      <c r="C36" s="31">
+      <c r="C36" s="53">
         <v>35359</v>
       </c>
       <c r="D36" s="22">
@@ -20041,8 +20068,8 @@
       <c r="B37" s="4">
         <v>1997</v>
       </c>
-      <c r="C37" s="31" t="s">
-        <v>70</v>
+      <c r="C37" s="53">
+        <v>35506</v>
       </c>
       <c r="D37" s="22">
         <v>43466</v>
@@ -20089,7 +20116,7 @@
       <c r="B38" s="4">
         <v>1997</v>
       </c>
-      <c r="C38" s="22">
+      <c r="C38" s="51">
         <v>35548</v>
       </c>
       <c r="D38" s="22">
@@ -20137,7 +20164,7 @@
       <c r="B39" s="4">
         <v>1997</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C39" s="51">
         <v>35632</v>
       </c>
       <c r="D39" s="22">
@@ -20185,7 +20212,7 @@
       <c r="B40" s="4">
         <v>1997</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C40" s="51">
         <v>35695</v>
       </c>
       <c r="D40" s="22">
@@ -20233,7 +20260,7 @@
       <c r="B41" s="4">
         <v>1997</v>
       </c>
-      <c r="C41" s="22">
+      <c r="C41" s="51">
         <v>35730</v>
       </c>
       <c r="D41" s="22">
@@ -20281,8 +20308,8 @@
       <c r="B42" s="4">
         <v>1998</v>
       </c>
-      <c r="C42" s="31" t="s">
-        <v>248</v>
+      <c r="C42" s="53">
+        <v>35803</v>
       </c>
       <c r="D42" s="22">
         <v>43466</v>
@@ -20329,7 +20356,7 @@
       <c r="B43" s="4">
         <v>1998</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C43" s="51">
         <v>35871</v>
       </c>
       <c r="D43" s="22">
@@ -20377,8 +20404,8 @@
       <c r="B44" s="4">
         <v>1998</v>
       </c>
-      <c r="C44" s="31" t="s">
-        <v>84</v>
+      <c r="C44" s="53">
+        <v>35871</v>
       </c>
       <c r="D44" s="22">
         <v>43466</v>
@@ -20425,8 +20452,8 @@
       <c r="B45" s="4">
         <v>1998</v>
       </c>
-      <c r="C45" s="22" t="s">
-        <v>89</v>
+      <c r="C45" s="51">
+        <v>35936</v>
       </c>
       <c r="D45" s="22">
         <v>43466</v>
@@ -20473,7 +20500,7 @@
       <c r="B46" s="4">
         <v>1998</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="51">
         <v>36060</v>
       </c>
       <c r="D46" s="22">
@@ -20521,7 +20548,7 @@
       <c r="B47" s="4">
         <v>1999</v>
       </c>
-      <c r="C47" s="22">
+      <c r="C47" s="51">
         <v>36171</v>
       </c>
       <c r="D47" s="22">
@@ -20569,8 +20596,8 @@
       <c r="B48" s="4">
         <v>1999</v>
       </c>
-      <c r="C48" s="31" t="s">
-        <v>96</v>
+      <c r="C48" s="53">
+        <v>36248</v>
       </c>
       <c r="D48" s="22">
         <v>43466</v>
@@ -20617,7 +20644,7 @@
       <c r="B49" s="4">
         <v>1999</v>
       </c>
-      <c r="C49" s="22">
+      <c r="C49" s="51">
         <v>36255</v>
       </c>
       <c r="D49" s="22">
@@ -20665,7 +20692,7 @@
       <c r="B50" s="4">
         <v>2000</v>
       </c>
-      <c r="C50" s="22">
+      <c r="C50" s="51">
         <v>36543</v>
       </c>
       <c r="D50" s="22">
@@ -20713,8 +20740,8 @@
       <c r="B51" s="4">
         <v>2000</v>
       </c>
-      <c r="C51" s="31" t="s">
-        <v>103</v>
+      <c r="C51" s="53">
+        <v>36544</v>
       </c>
       <c r="D51" s="22">
         <v>43466</v>
@@ -20761,8 +20788,8 @@
       <c r="B52" s="4">
         <v>2000</v>
       </c>
-      <c r="C52" s="31" t="s">
-        <v>103</v>
+      <c r="C52" s="53">
+        <v>36544</v>
       </c>
       <c r="D52" s="22">
         <v>43466</v>
@@ -20809,8 +20836,8 @@
       <c r="B53" s="4">
         <v>2000</v>
       </c>
-      <c r="C53" s="31" t="s">
-        <v>109</v>
+      <c r="C53" s="53">
+        <v>36794</v>
       </c>
       <c r="D53" s="22">
         <v>43466</v>
@@ -20857,8 +20884,8 @@
       <c r="B54" s="4">
         <v>2000</v>
       </c>
-      <c r="C54" s="31" t="s">
-        <v>249</v>
+      <c r="C54" s="53">
+        <v>36822</v>
       </c>
       <c r="D54" s="22">
         <v>43466</v>
@@ -20905,8 +20932,8 @@
       <c r="B55" s="4">
         <v>2000</v>
       </c>
-      <c r="C55" s="31" t="s">
-        <v>115</v>
+      <c r="C55" s="53">
+        <v>36857</v>
       </c>
       <c r="D55" s="22">
         <v>43466</v>
@@ -20953,7 +20980,7 @@
       <c r="B56" s="4">
         <v>2000</v>
       </c>
-      <c r="C56" s="22">
+      <c r="C56" s="51">
         <v>36857</v>
       </c>
       <c r="D56" s="22">
@@ -21001,7 +21028,7 @@
       <c r="B57" s="4">
         <v>2000</v>
       </c>
-      <c r="C57" s="22">
+      <c r="C57" s="51">
         <v>36860</v>
       </c>
       <c r="D57" s="22">
@@ -21049,7 +21076,7 @@
       <c r="B58" s="4">
         <v>2000</v>
       </c>
-      <c r="C58" s="22">
+      <c r="C58" s="51">
         <v>36873</v>
       </c>
       <c r="D58" s="22">
@@ -21097,7 +21124,7 @@
       <c r="B59" s="4">
         <v>2001</v>
       </c>
-      <c r="C59" s="22">
+      <c r="C59" s="51">
         <v>37202</v>
       </c>
       <c r="D59" s="22">
@@ -21145,8 +21172,8 @@
       <c r="B60" s="4">
         <v>2003</v>
       </c>
-      <c r="C60" s="30" t="s">
-        <v>124</v>
+      <c r="C60" s="52">
+        <v>37662</v>
       </c>
       <c r="D60" s="22">
         <v>43466</v>
@@ -21193,7 +21220,7 @@
       <c r="B61" s="4">
         <v>2005</v>
       </c>
-      <c r="C61" s="30">
+      <c r="C61" s="52">
         <v>38636</v>
       </c>
       <c r="D61" s="22">
@@ -21241,7 +21268,7 @@
       <c r="B62" s="4">
         <v>2006</v>
       </c>
-      <c r="C62" s="32">
+      <c r="C62" s="54">
         <v>39009</v>
       </c>
       <c r="D62" s="22">
@@ -21289,7 +21316,7 @@
       <c r="B63" s="4">
         <v>2006</v>
       </c>
-      <c r="C63" s="22">
+      <c r="C63" s="51">
         <v>39062</v>
       </c>
       <c r="D63" s="22">
@@ -21337,8 +21364,8 @@
       <c r="B64" s="4">
         <v>2007</v>
       </c>
-      <c r="C64" s="31" t="s">
-        <v>251</v>
+      <c r="C64" s="53">
+        <v>39146</v>
       </c>
       <c r="D64" s="22">
         <v>43466</v>
@@ -21385,8 +21412,8 @@
       <c r="B65" s="4">
         <v>2007</v>
       </c>
-      <c r="C65" s="22" t="s">
-        <v>252</v>
+      <c r="C65" s="51">
+        <v>39160</v>
       </c>
       <c r="D65" s="22">
         <v>43466</v>
@@ -21433,8 +21460,8 @@
       <c r="B66" s="4">
         <v>2007</v>
       </c>
-      <c r="C66" s="31" t="s">
-        <v>253</v>
+      <c r="C66" s="53">
+        <v>39181</v>
       </c>
       <c r="D66" s="22">
         <v>43466</v>
@@ -21481,8 +21508,8 @@
       <c r="B67" s="4">
         <v>2007</v>
       </c>
-      <c r="C67" s="31" t="s">
-        <v>254</v>
+      <c r="C67" s="53">
+        <v>39293</v>
       </c>
       <c r="D67" s="22">
         <v>43466</v>
@@ -21529,7 +21556,7 @@
       <c r="B68" s="4">
         <v>2007</v>
       </c>
-      <c r="C68" s="22">
+      <c r="C68" s="51">
         <v>39314</v>
       </c>
       <c r="D68" s="22">
@@ -21577,8 +21604,8 @@
       <c r="B69" s="4">
         <v>2007</v>
       </c>
-      <c r="C69" s="31" t="s">
-        <v>255</v>
+      <c r="C69" s="53">
+        <v>39419</v>
       </c>
       <c r="D69" s="22">
         <v>43466</v>
@@ -21625,7 +21652,7 @@
       <c r="B70" s="4">
         <v>2008</v>
       </c>
-      <c r="C70" s="22">
+      <c r="C70" s="51">
         <v>39454</v>
       </c>
       <c r="D70" s="22">
@@ -21673,8 +21700,8 @@
       <c r="B71" s="4">
         <v>2008</v>
       </c>
-      <c r="C71" s="22" t="s">
-        <v>256</v>
+      <c r="C71" s="51">
+        <v>39468</v>
       </c>
       <c r="D71" s="22">
         <v>43466</v>
@@ -21721,8 +21748,8 @@
       <c r="B72" s="4">
         <v>2008</v>
       </c>
-      <c r="C72" s="31" t="s">
-        <v>257</v>
+      <c r="C72" s="53">
+        <v>39693</v>
       </c>
       <c r="D72" s="22">
         <v>43466</v>
@@ -21769,8 +21796,8 @@
       <c r="B73" s="4">
         <v>2008</v>
       </c>
-      <c r="C73" s="31" t="s">
-        <v>141</v>
+      <c r="C73" s="53">
+        <v>39769</v>
       </c>
       <c r="D73" s="22">
         <v>43466</v>
@@ -21817,7 +21844,7 @@
       <c r="B74" s="4">
         <v>2010</v>
       </c>
-      <c r="C74" s="22">
+      <c r="C74" s="51">
         <v>40399</v>
       </c>
       <c r="D74" s="22">
@@ -21865,7 +21892,7 @@
       <c r="B75" s="4">
         <v>2010</v>
       </c>
-      <c r="C75" s="22">
+      <c r="C75" s="51">
         <v>40399</v>
       </c>
       <c r="D75" s="22">
@@ -21913,7 +21940,7 @@
       <c r="B76" s="4">
         <v>2010</v>
       </c>
-      <c r="C76" s="22">
+      <c r="C76" s="51">
         <v>40399</v>
       </c>
       <c r="D76" s="22">
@@ -21961,8 +21988,8 @@
       <c r="B77" s="4">
         <v>2010</v>
       </c>
-      <c r="C77" s="31" t="s">
-        <v>258</v>
+      <c r="C77" s="53">
+        <v>40399</v>
       </c>
       <c r="D77" s="22">
         <v>43466</v>
@@ -22009,7 +22036,7 @@
       <c r="B78" s="4">
         <v>2010</v>
       </c>
-      <c r="C78" s="22">
+      <c r="C78" s="51">
         <v>40406</v>
       </c>
       <c r="D78" s="22">
@@ -22057,7 +22084,7 @@
       <c r="B79" s="4">
         <v>2010</v>
       </c>
-      <c r="C79" s="22">
+      <c r="C79" s="51">
         <v>40406</v>
       </c>
       <c r="D79" s="22">
@@ -22105,7 +22132,7 @@
       <c r="B80" s="4">
         <v>2010</v>
       </c>
-      <c r="C80" s="22">
+      <c r="C80" s="51">
         <v>40406</v>
       </c>
       <c r="D80" s="22">
@@ -22153,7 +22180,7 @@
       <c r="B81" s="4">
         <v>2010</v>
       </c>
-      <c r="C81" s="22">
+      <c r="C81" s="51">
         <v>40406</v>
       </c>
       <c r="D81" s="22">
@@ -22201,8 +22228,8 @@
       <c r="B82" s="4">
         <v>2010</v>
       </c>
-      <c r="C82" s="31" t="s">
-        <v>259</v>
+      <c r="C82" s="53">
+        <v>40420</v>
       </c>
       <c r="D82" s="22">
         <v>43466</v>
@@ -22249,8 +22276,8 @@
       <c r="B83" s="4">
         <v>2011</v>
       </c>
-      <c r="C83" s="31" t="s">
-        <v>201</v>
+      <c r="C83" s="53">
+        <v>40875</v>
       </c>
       <c r="D83" s="22">
         <v>43466</v>
@@ -22297,8 +22324,8 @@
       <c r="B84" s="4">
         <v>2011</v>
       </c>
-      <c r="C84" s="31" t="s">
-        <v>260</v>
+      <c r="C84" s="53">
+        <v>40770</v>
       </c>
       <c r="D84" s="22">
         <v>43466</v>
@@ -22345,7 +22372,7 @@
       <c r="B85" s="4">
         <v>2011</v>
       </c>
-      <c r="C85" s="22">
+      <c r="C85" s="51">
         <v>40777</v>
       </c>
       <c r="D85" s="22">
@@ -22393,8 +22420,8 @@
       <c r="B86" s="4">
         <v>2011</v>
       </c>
-      <c r="C86" s="31" t="s">
-        <v>261</v>
+      <c r="C86" s="53">
+        <v>40777</v>
       </c>
       <c r="D86" s="22">
         <v>43466</v>
@@ -22441,8 +22468,8 @@
       <c r="B87" s="4">
         <v>2011</v>
       </c>
-      <c r="C87" s="22" t="s">
-        <v>262</v>
+      <c r="C87" s="51">
+        <v>40792</v>
       </c>
       <c r="D87" s="22">
         <v>43466</v>
@@ -22489,7 +22516,7 @@
       <c r="B88" s="4">
         <v>2011</v>
       </c>
-      <c r="C88" s="22">
+      <c r="C88" s="51">
         <v>40812</v>
       </c>
       <c r="D88" s="22">
@@ -22537,8 +22564,8 @@
       <c r="B89" s="4">
         <v>2011</v>
       </c>
-      <c r="C89" s="31" t="s">
-        <v>173</v>
+      <c r="C89" s="53">
+        <v>40833</v>
       </c>
       <c r="D89" s="22">
         <v>43466</v>
@@ -22585,8 +22612,8 @@
       <c r="B90" s="4">
         <v>2011</v>
       </c>
-      <c r="C90" s="22" t="s">
-        <v>176</v>
+      <c r="C90" s="51">
+        <v>40840</v>
       </c>
       <c r="D90" s="22">
         <v>43466</v>
@@ -22633,7 +22660,7 @@
       <c r="B91" s="4">
         <v>2011</v>
       </c>
-      <c r="C91" s="22">
+      <c r="C91" s="51">
         <v>40840</v>
       </c>
       <c r="D91" s="22">
@@ -22681,8 +22708,8 @@
       <c r="B92" s="4">
         <v>2011</v>
       </c>
-      <c r="C92" s="31" t="s">
-        <v>176</v>
+      <c r="C92" s="53">
+        <v>40840</v>
       </c>
       <c r="D92" s="22">
         <v>43466</v>
@@ -22729,8 +22756,8 @@
       <c r="B93" s="4">
         <v>2011</v>
       </c>
-      <c r="C93" s="31" t="s">
-        <v>183</v>
+      <c r="C93" s="53">
+        <v>40847</v>
       </c>
       <c r="D93" s="22">
         <v>43466</v>
@@ -22777,7 +22804,7 @@
       <c r="B94" s="4">
         <v>2011</v>
       </c>
-      <c r="C94" s="30">
+      <c r="C94" s="52">
         <v>40847</v>
       </c>
       <c r="D94" s="22">
@@ -22825,7 +22852,7 @@
       <c r="B95" s="4">
         <v>2011</v>
       </c>
-      <c r="C95" s="22">
+      <c r="C95" s="51">
         <v>40854</v>
       </c>
       <c r="D95" s="22">
@@ -22873,8 +22900,8 @@
       <c r="B96" s="4">
         <v>2011</v>
       </c>
-      <c r="C96" s="31" t="s">
-        <v>263</v>
+      <c r="C96" s="53">
+        <v>40854</v>
       </c>
       <c r="D96" s="22">
         <v>43466</v>
@@ -22921,8 +22948,8 @@
       <c r="B97" s="4">
         <v>2011</v>
       </c>
-      <c r="C97" s="31" t="s">
-        <v>263</v>
+      <c r="C97" s="53">
+        <v>40854</v>
       </c>
       <c r="D97" s="22">
         <v>43466</v>
@@ -22969,8 +22996,8 @@
       <c r="B98" s="4">
         <v>2011</v>
       </c>
-      <c r="C98" s="31" t="s">
-        <v>263</v>
+      <c r="C98" s="53">
+        <v>40854</v>
       </c>
       <c r="D98" s="22">
         <v>43466</v>
@@ -23017,8 +23044,8 @@
       <c r="B99" s="4">
         <v>2011</v>
       </c>
-      <c r="C99" s="31" t="s">
-        <v>195</v>
+      <c r="C99" s="53">
+        <v>40861</v>
       </c>
       <c r="D99" s="22">
         <v>43466</v>
@@ -23065,8 +23092,8 @@
       <c r="B100" s="4">
         <v>2011</v>
       </c>
-      <c r="C100" s="22" t="s">
-        <v>198</v>
+      <c r="C100" s="51">
+        <v>40868</v>
       </c>
       <c r="D100" s="22">
         <v>43466</v>
@@ -23113,7 +23140,7 @@
       <c r="B101" s="4">
         <v>2011</v>
       </c>
-      <c r="C101" s="22">
+      <c r="C101" s="51">
         <v>40875</v>
       </c>
       <c r="D101" s="22">
@@ -23161,8 +23188,8 @@
       <c r="B102" s="4">
         <v>2011</v>
       </c>
-      <c r="C102" s="31" t="s">
-        <v>201</v>
+      <c r="C102" s="53">
+        <v>40875</v>
       </c>
       <c r="D102" s="22">
         <v>43466</v>
@@ -23209,8 +23236,8 @@
       <c r="B103" s="4">
         <v>2012</v>
       </c>
-      <c r="C103" s="31" t="s">
-        <v>264</v>
+      <c r="C103" s="53">
+        <v>40911</v>
       </c>
       <c r="D103" s="22">
         <v>43466</v>
@@ -23257,8 +23284,8 @@
       <c r="B104" s="4">
         <v>2012</v>
       </c>
-      <c r="C104" s="31" t="s">
-        <v>264</v>
+      <c r="C104" s="53">
+        <v>40911</v>
       </c>
       <c r="D104" s="22">
         <v>43466</v>
@@ -23305,7 +23332,7 @@
       <c r="B105" s="4">
         <v>2012</v>
       </c>
-      <c r="C105" s="22">
+      <c r="C105" s="51">
         <v>40911</v>
       </c>
       <c r="D105" s="22">
@@ -23353,7 +23380,7 @@
       <c r="B106" s="4">
         <v>2012</v>
       </c>
-      <c r="C106" s="22">
+      <c r="C106" s="51">
         <v>40924</v>
       </c>
       <c r="D106" s="22">
@@ -23401,8 +23428,8 @@
       <c r="B107" s="4">
         <v>2012</v>
       </c>
-      <c r="C107" s="22" t="s">
-        <v>265</v>
+      <c r="C107" s="51">
+        <v>40931</v>
       </c>
       <c r="D107" s="22">
         <v>43466</v>
@@ -23449,7 +23476,7 @@
       <c r="B108" s="4">
         <v>2012</v>
       </c>
-      <c r="C108" s="22">
+      <c r="C108" s="51">
         <v>41085</v>
       </c>
       <c r="D108" s="22">
@@ -23497,8 +23524,8 @@
       <c r="B109" s="4">
         <v>2012</v>
       </c>
-      <c r="C109" s="31" t="s">
-        <v>266</v>
+      <c r="C109" s="53">
+        <v>41106</v>
       </c>
       <c r="D109" s="22">
         <v>43466</v>
@@ -23545,8 +23572,8 @@
       <c r="B110" s="4">
         <v>2012</v>
       </c>
-      <c r="C110" s="31" t="s">
-        <v>267</v>
+      <c r="C110" s="53">
+        <v>41120</v>
       </c>
       <c r="D110" s="22">
         <v>43466</v>
@@ -23593,7 +23620,7 @@
       <c r="B111" s="4">
         <v>2012</v>
       </c>
-      <c r="C111" s="31">
+      <c r="C111" s="53">
         <v>41127</v>
       </c>
       <c r="D111" s="22">
@@ -23641,8 +23668,8 @@
       <c r="B112" s="4">
         <v>2012</v>
       </c>
-      <c r="C112" s="31" t="s">
-        <v>268</v>
+      <c r="C112" s="53">
+        <v>41127</v>
       </c>
       <c r="D112" s="22">
         <v>43466</v>
@@ -23689,8 +23716,8 @@
       <c r="B113" s="4">
         <v>2012</v>
       </c>
-      <c r="C113" s="31" t="s">
-        <v>269</v>
+      <c r="C113" s="53">
+        <v>41134</v>
       </c>
       <c r="D113" s="22">
         <v>43466</v>
@@ -23737,8 +23764,8 @@
       <c r="B114" s="4">
         <v>2012</v>
       </c>
-      <c r="C114" s="31" t="s">
-        <v>270</v>
+      <c r="C114" s="53">
+        <v>41176</v>
       </c>
       <c r="D114" s="22">
         <v>43466</v>
@@ -23785,8 +23812,8 @@
       <c r="B115" s="4">
         <v>2012</v>
       </c>
-      <c r="C115" s="31" t="s">
-        <v>270</v>
+      <c r="C115" s="53">
+        <v>41176</v>
       </c>
       <c r="D115" s="22">
         <v>43466</v>
@@ -23833,7 +23860,7 @@
       <c r="B116" s="4">
         <v>2012</v>
       </c>
-      <c r="C116" s="22">
+      <c r="C116" s="51">
         <v>41211</v>
       </c>
       <c r="D116" s="22">
@@ -23881,7 +23908,7 @@
       <c r="B117" s="4">
         <v>2013</v>
       </c>
-      <c r="C117" s="22">
+      <c r="C117" s="51">
         <v>41302</v>
       </c>
       <c r="D117" s="22">
@@ -23929,8 +23956,8 @@
       <c r="B118" s="4">
         <v>2013</v>
       </c>
-      <c r="C118" s="31" t="s">
-        <v>271</v>
+      <c r="C118" s="53">
+        <v>41309</v>
       </c>
       <c r="D118" s="22">
         <v>43466</v>
@@ -23977,7 +24004,7 @@
       <c r="B119" s="4">
         <v>2013</v>
       </c>
-      <c r="C119" s="22">
+      <c r="C119" s="51">
         <v>41316</v>
       </c>
       <c r="D119" s="22">
@@ -24025,8 +24052,8 @@
       <c r="B120" s="4">
         <v>2013</v>
       </c>
-      <c r="C120" s="31" t="s">
-        <v>272</v>
+      <c r="C120" s="53">
+        <v>41316</v>
       </c>
       <c r="D120" s="22">
         <v>43466</v>
@@ -24073,8 +24100,8 @@
       <c r="B121" s="4">
         <v>2013</v>
       </c>
-      <c r="C121" s="31" t="s">
-        <v>274</v>
+      <c r="C121" s="53">
+        <v>41379</v>
       </c>
       <c r="D121" s="22">
         <v>43466</v>
@@ -24121,8 +24148,8 @@
       <c r="B122" s="4">
         <v>2013</v>
       </c>
-      <c r="C122" s="31" t="s">
-        <v>277</v>
+      <c r="C122" s="53">
+        <v>41386</v>
       </c>
       <c r="D122" s="22">
         <v>43466</v>
@@ -24169,8 +24196,8 @@
       <c r="B123" s="4">
         <v>2013</v>
       </c>
-      <c r="C123" s="31" t="s">
-        <v>286</v>
+      <c r="C123" s="53">
+        <v>41407</v>
       </c>
       <c r="D123" s="22">
         <v>43466</v>
@@ -24217,8 +24244,8 @@
       <c r="B124" s="4">
         <v>2013</v>
       </c>
-      <c r="C124" s="31" t="s">
-        <v>282</v>
+      <c r="C124" s="53">
+        <v>41414</v>
       </c>
       <c r="D124" s="22">
         <v>43466</v>
@@ -24265,8 +24292,8 @@
       <c r="B125" s="4">
         <v>2013</v>
       </c>
-      <c r="C125" s="31" t="s">
-        <v>283</v>
+      <c r="C125" s="53">
+        <v>41422</v>
       </c>
       <c r="D125" s="22">
         <v>43466</v>
@@ -24313,7 +24340,7 @@
       <c r="B126" s="4">
         <v>2013</v>
       </c>
-      <c r="C126" s="31">
+      <c r="C126" s="53">
         <v>41422</v>
       </c>
       <c r="D126" s="22">
@@ -24361,7 +24388,7 @@
       <c r="B127" s="4">
         <v>2013</v>
       </c>
-      <c r="C127" s="31">
+      <c r="C127" s="53">
         <v>41449</v>
       </c>
       <c r="D127" s="22">
@@ -24409,7 +24436,7 @@
       <c r="B128" s="4">
         <v>2013</v>
       </c>
-      <c r="C128" s="31">
+      <c r="C128" s="53">
         <v>41449</v>
       </c>
       <c r="D128" s="22">
@@ -24457,7 +24484,7 @@
       <c r="B129" s="4">
         <v>2013</v>
       </c>
-      <c r="C129" s="31">
+      <c r="C129" s="53">
         <v>41449</v>
       </c>
       <c r="D129" s="22">
@@ -24505,7 +24532,7 @@
       <c r="B130" s="4">
         <v>2013</v>
       </c>
-      <c r="C130" s="31">
+      <c r="C130" s="53">
         <v>41463</v>
       </c>
       <c r="D130" s="22">
@@ -24553,7 +24580,7 @@
       <c r="B131" s="4">
         <v>2013</v>
       </c>
-      <c r="C131" s="31">
+      <c r="C131" s="53">
         <v>41491</v>
       </c>
       <c r="D131" s="22">
@@ -24601,7 +24628,7 @@
       <c r="B132" s="4">
         <v>2013</v>
       </c>
-      <c r="C132" s="31">
+      <c r="C132" s="53">
         <v>41491</v>
       </c>
       <c r="D132" s="22">
@@ -24649,7 +24676,7 @@
       <c r="B133" s="4">
         <v>2013</v>
       </c>
-      <c r="C133" s="31">
+      <c r="C133" s="53">
         <v>41498</v>
       </c>
       <c r="D133" s="22">
@@ -24697,7 +24724,7 @@
       <c r="B134" s="4">
         <v>2013</v>
       </c>
-      <c r="C134" s="31">
+      <c r="C134" s="53">
         <v>41498</v>
       </c>
       <c r="D134" s="22">
@@ -24745,7 +24772,7 @@
       <c r="B135" s="4">
         <v>2013</v>
       </c>
-      <c r="C135" s="31">
+      <c r="C135" s="53">
         <v>41505</v>
       </c>
       <c r="D135" s="22">
@@ -24793,7 +24820,7 @@
       <c r="B136" s="4">
         <v>2013</v>
       </c>
-      <c r="C136" s="31">
+      <c r="C136" s="53">
         <v>41505</v>
       </c>
       <c r="D136" s="22">
@@ -24841,7 +24868,7 @@
       <c r="B137" s="4">
         <v>2013</v>
       </c>
-      <c r="C137" s="31">
+      <c r="C137" s="53">
         <v>41505</v>
       </c>
       <c r="D137" s="22">
@@ -24889,7 +24916,7 @@
       <c r="B138" s="4">
         <v>2013</v>
       </c>
-      <c r="C138" s="31">
+      <c r="C138" s="53">
         <v>41526</v>
       </c>
       <c r="D138" s="22">
@@ -24937,7 +24964,7 @@
       <c r="B139" s="4">
         <v>2013</v>
       </c>
-      <c r="C139" s="31">
+      <c r="C139" s="53">
         <v>41568</v>
       </c>
       <c r="D139" s="22">
@@ -24985,7 +25012,7 @@
       <c r="B140" s="4">
         <v>2013</v>
       </c>
-      <c r="C140" s="31">
+      <c r="C140" s="53">
         <v>41575</v>
       </c>
       <c r="D140" s="22">
@@ -25033,7 +25060,7 @@
       <c r="B141" s="4">
         <v>2013</v>
       </c>
-      <c r="C141" s="31">
+      <c r="C141" s="53">
         <v>41582</v>
       </c>
       <c r="D141" s="22">
@@ -25081,7 +25108,7 @@
       <c r="B142" s="4">
         <v>2013</v>
       </c>
-      <c r="C142" s="31">
+      <c r="C142" s="53">
         <v>41589</v>
       </c>
       <c r="D142" s="22">
@@ -25129,7 +25156,7 @@
       <c r="B143" s="4">
         <v>2013</v>
       </c>
-      <c r="C143" s="31">
+      <c r="C143" s="53">
         <v>41589</v>
       </c>
       <c r="D143" s="22">
@@ -25177,7 +25204,7 @@
       <c r="B144" s="4">
         <v>2013</v>
       </c>
-      <c r="C144" s="31">
+      <c r="C144" s="53">
         <v>41589</v>
       </c>
       <c r="D144" s="22">
@@ -25225,7 +25252,7 @@
       <c r="B145" s="4">
         <v>2013</v>
       </c>
-      <c r="C145" s="31">
+      <c r="C145" s="53">
         <v>41596</v>
       </c>
       <c r="D145" s="22">
@@ -25273,7 +25300,7 @@
       <c r="B146" s="4">
         <v>2013</v>
       </c>
-      <c r="C146" s="31">
+      <c r="C146" s="53">
         <v>41596</v>
       </c>
       <c r="D146" s="22">
@@ -25321,7 +25348,7 @@
       <c r="B147" s="4">
         <v>2013</v>
       </c>
-      <c r="C147" s="31">
+      <c r="C147" s="53">
         <v>41610</v>
       </c>
       <c r="D147" s="22">
@@ -25369,7 +25396,7 @@
       <c r="B148" s="4">
         <v>2013</v>
       </c>
-      <c r="C148" s="31">
+      <c r="C148" s="53">
         <v>41610</v>
       </c>
       <c r="D148" s="22">
@@ -25417,7 +25444,7 @@
       <c r="B149" s="4">
         <v>2013</v>
       </c>
-      <c r="C149" s="31">
+      <c r="C149" s="53">
         <v>41610</v>
       </c>
       <c r="D149" s="22">
@@ -25465,7 +25492,7 @@
       <c r="B150" s="4">
         <v>2013</v>
       </c>
-      <c r="C150" s="31">
+      <c r="C150" s="53">
         <v>41610</v>
       </c>
       <c r="D150" s="22">
@@ -25513,7 +25540,7 @@
       <c r="B151" s="4">
         <v>2013</v>
       </c>
-      <c r="C151" s="31">
+      <c r="C151" s="53">
         <v>41610</v>
       </c>
       <c r="D151" s="22">
@@ -25561,7 +25588,7 @@
       <c r="B152" s="4">
         <v>2013</v>
       </c>
-      <c r="C152" s="31">
+      <c r="C152" s="53">
         <v>41610</v>
       </c>
       <c r="D152" s="22">
@@ -25609,7 +25636,7 @@
       <c r="B153" s="4">
         <v>2013</v>
       </c>
-      <c r="C153" s="31">
+      <c r="C153" s="53">
         <v>41617</v>
       </c>
       <c r="D153" s="22">
@@ -32150,7 +32177,9 @@
       <c r="H289" s="29" t="s">
         <v>497</v>
       </c>
-      <c r="I289" s="24"/>
+      <c r="I289" s="24">
+        <v>0</v>
+      </c>
       <c r="J289" s="25">
         <f>IFERROR(VLOOKUP(H289,#REF!,2,FALSE),0)</f>
         <v>0</v>
@@ -32195,7 +32224,9 @@
       <c r="H290" s="29" t="s">
         <v>527</v>
       </c>
-      <c r="I290" s="24"/>
+      <c r="I290" s="24">
+        <v>0</v>
+      </c>
       <c r="J290" s="25">
         <f>IFERROR(VLOOKUP(H290,#REF!,2,FALSE),0)</f>
         <v>0</v>
@@ -32334,7 +32365,9 @@
       <c r="H293" s="5" t="s">
         <v>618</v>
       </c>
-      <c r="I293" s="24"/>
+      <c r="I293" s="24">
+        <v>0</v>
+      </c>
       <c r="J293" s="25">
         <f>IFERROR(VLOOKUP(H293,#REF!,2,FALSE),0)</f>
         <v>0</v>
@@ -32661,7 +32694,9 @@
       <c r="H300" s="8" t="s">
         <v>768</v>
       </c>
-      <c r="I300" s="24"/>
+      <c r="I300" s="24">
+        <v>0</v>
+      </c>
       <c r="J300" s="25">
         <f>IFERROR(VLOOKUP(H300,#REF!,2,FALSE),0)</f>
         <v>0</v>
@@ -32801,7 +32836,9 @@
       <c r="H303" s="8" t="s">
         <v>762</v>
       </c>
-      <c r="I303" s="24"/>
+      <c r="I303" s="24">
+        <v>0</v>
+      </c>
       <c r="J303" s="25">
         <f>IFERROR(VLOOKUP(H303,#REF!,2,FALSE),0)</f>
         <v>0</v>
@@ -32821,6 +32858,7 @@
       </c>
       <c r="O303" s="8"/>
     </row>
+    <row r="304" spans="1:15" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>